<commit_message>
Repeat microarray experiments with min-max norm
</commit_message>
<xml_diff>
--- a/experiment_plans/large_upper_ex_plan.xlsx
+++ b/experiment_plans/large_upper_ex_plan.xlsx
@@ -2192,7 +2192,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -2201,31 +2201,31 @@
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>8</v>
@@ -2236,13 +2236,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -2251,25 +2251,25 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>9</v>
@@ -2280,19 +2280,19 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
@@ -2301,19 +2301,19 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>10</v>
@@ -2324,25 +2324,25 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>11</v>
@@ -2351,13 +2351,13 @@
         <v>11</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>11</v>
@@ -4748,7 +4748,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
         <v>2</v>

</xml_diff>